<commit_message>
abis pre processing, progress cek catetan
</commit_message>
<xml_diff>
--- a/Tren Penerimaan MABA UMP 2014 - 2024/dataset/jumlah missing values.xlsx
+++ b/Tren Penerimaan MABA UMP 2014 - 2024/dataset/jumlah missing values.xlsx
@@ -249,7 +249,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,13 +259,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -323,7 +317,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -652,7 +646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -660,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -668,7 +662,7 @@
         <v>65954</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -676,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -684,7 +678,7 @@
         <v>25139</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -692,7 +686,7 @@
         <v>25139</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -700,7 +694,7 @@
         <v>25139</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -708,7 +702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -716,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -724,7 +718,7 @@
         <v>65954</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -732,7 +726,7 @@
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -740,7 +734,7 @@
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -748,7 +742,7 @@
         <v>20233</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -756,7 +750,7 @@
         <v>20233</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -764,7 +758,7 @@
         <v>7537</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -772,7 +766,7 @@
         <v>7537</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -780,7 +774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
@@ -788,7 +782,7 @@
         <v>27684</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
@@ -796,7 +790,7 @@
         <v>58962</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -804,7 +798,7 @@
         <v>65954</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -812,7 +806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
@@ -820,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
@@ -828,7 +822,7 @@
         <v>25147</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
@@ -836,7 +830,7 @@
         <v>25144</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
@@ -844,7 +838,7 @@
         <v>33779</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3" t="s">
         <v>26</v>
       </c>

</xml_diff>